<commit_message>
feat: version stable des projets forum des métiers 2024
</commit_message>
<xml_diff>
--- a/comparatif.xlsx
+++ b/comparatif.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\didie\Documents\ws\demo-rpa\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2D6ECE2-36F6-490D-BEB6-2D95BC77F581}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{16E3A364-75E1-432C-8C1D-FDBB67E48A15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Influencers" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="24">
   <si>
     <t>Influenceur 1</t>
   </si>
@@ -460,6 +460,21 @@
     <xf numFmtId="0" fontId="10" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -477,21 +492,6 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -611,21 +611,13 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Comparatif!$C$3:$G$3</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>michou</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>bigfloetoly</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>inoxtag</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -633,15 +625,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>1700000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>166</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -676,21 +659,13 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Comparatif!$C$3:$G$3</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>michou</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>bigfloetoly</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>inoxtag</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -698,15 +673,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>9400000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>3080000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7210000</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -741,21 +707,13 @@
           </c:spPr>
           <c:invertIfNegative val="0"/>
           <c:cat>
-            <c:strRef>
+            <c:numRef>
               <c:f>Comparatif!$C$3:$G$3</c:f>
-              <c:strCache>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>michou</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>bigfloetoly</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>inoxtag</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+              </c:numCache>
+            </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
@@ -763,15 +721,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>4600000</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>2300000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>4800000</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
@@ -1826,22 +1775,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:O22"/>
+  <dimension ref="A1:AA36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="2.26953125" customWidth="1"/>
-    <col min="4" max="4" width="22.54296875" customWidth="1"/>
-    <col min="6" max="6" width="22.1796875" customWidth="1"/>
-    <col min="8" max="8" width="24.453125" customWidth="1"/>
-    <col min="9" max="9" width="3.08984375" customWidth="1"/>
+    <col min="3" max="3" width="2.21875" customWidth="1"/>
+    <col min="4" max="4" width="22.5546875" customWidth="1"/>
+    <col min="6" max="6" width="22.21875" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" customWidth="1"/>
+    <col min="9" max="9" width="3.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:27" ht="7.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -1858,17 +1807,17 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
     </row>
-    <row r="2" spans="1:15" ht="36.5" thickBot="1" x14ac:dyDescent="0.85">
+    <row r="2" spans="1:27" ht="37.200000000000003" thickBot="1" x14ac:dyDescent="0.75">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1"/>
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="37"/>
-      <c r="F2" s="37"/>
-      <c r="G2" s="37"/>
-      <c r="H2" s="38"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
+      <c r="H2" s="43"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -1876,8 +1825,20 @@
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" ht="8.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P2" s="1"/>
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+      <c r="Z2" s="1"/>
+      <c r="AA2" s="1"/>
+    </row>
+    <row r="3" spans="1:27" ht="8.5500000000000007" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1893,8 +1854,20 @@
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
-    </row>
-    <row r="4" spans="1:15" ht="8" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P3" s="1"/>
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+      <c r="Z3" s="1"/>
+      <c r="AA3" s="1"/>
+    </row>
+    <row r="4" spans="1:27" ht="7.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1910,8 +1883,20 @@
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
-    </row>
-    <row r="5" spans="1:15" ht="26.5" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="P4" s="1"/>
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+      <c r="Z4" s="1"/>
+      <c r="AA4" s="1"/>
+    </row>
+    <row r="5" spans="1:27" ht="26.4" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1933,16 +1918,28 @@
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
-    </row>
-    <row r="6" spans="1:15" ht="14" customHeight="1" x14ac:dyDescent="0.6">
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+      <c r="Z5" s="1"/>
+      <c r="AA5" s="1"/>
+    </row>
+    <row r="6" spans="1:27" ht="13.95" customHeight="1" x14ac:dyDescent="0.5">
       <c r="A6" s="1"/>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="43"/>
-      <c r="F6" s="43"/>
-      <c r="G6" s="43"/>
-      <c r="H6" s="44"/>
+      <c r="D6" s="36"/>
+      <c r="E6" s="37"/>
+      <c r="F6" s="37"/>
+      <c r="G6" s="37"/>
+      <c r="H6" s="38"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
       <c r="K6" s="1"/>
@@ -1950,19 +1947,31 @@
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
-    </row>
-    <row r="7" spans="1:15" ht="26" x14ac:dyDescent="0.6">
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+      <c r="Z6" s="1"/>
+      <c r="AA6" s="1"/>
+    </row>
+    <row r="7" spans="1:27" ht="25.8" x14ac:dyDescent="0.5">
       <c r="A7" s="1"/>
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
       <c r="D7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45" t="s">
+      <c r="E7" s="39"/>
+      <c r="F7" s="39" t="s">
         <v>21</v>
       </c>
-      <c r="G7" s="45"/>
+      <c r="G7" s="39"/>
       <c r="H7" s="9" t="s">
         <v>13</v>
       </c>
@@ -1973,8 +1982,20 @@
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
-    </row>
-    <row r="8" spans="1:15" ht="9.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.65">
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+      <c r="Z7" s="1"/>
+      <c r="AA7" s="1"/>
+    </row>
+    <row r="8" spans="1:27" ht="9.4499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.55000000000000004">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -1990,8 +2011,20 @@
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
-    </row>
-    <row r="9" spans="1:15" ht="9.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+      <c r="Z8" s="1"/>
+      <c r="AA8" s="1"/>
+    </row>
+    <row r="9" spans="1:27" ht="9.4499999999999993" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2007,18 +2040,30 @@
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
-    </row>
-    <row r="10" spans="1:15" ht="23" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+      <c r="Z9" s="1"/>
+      <c r="AA9" s="1"/>
+    </row>
+    <row r="10" spans="1:27" ht="22.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
-      <c r="D10" s="39" t="s">
+      <c r="D10" s="44" t="s">
         <v>11</v>
       </c>
-      <c r="E10" s="40"/>
-      <c r="F10" s="40"/>
-      <c r="G10" s="40"/>
-      <c r="H10" s="41"/>
+      <c r="E10" s="45"/>
+      <c r="F10" s="45"/>
+      <c r="G10" s="45"/>
+      <c r="H10" s="46"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
       <c r="K10" s="1"/>
@@ -2026,8 +2071,20 @@
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
-    </row>
-    <row r="11" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+      <c r="Z10" s="1"/>
+      <c r="AA10" s="1"/>
+    </row>
+    <row r="11" spans="1:27" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2039,7 +2096,7 @@
         <v>14</v>
       </c>
       <c r="G11" s="32"/>
-      <c r="H11" s="46" t="s">
+      <c r="H11" s="40" t="s">
         <v>15</v>
       </c>
       <c r="I11" s="1"/>
@@ -2049,8 +2106,20 @@
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
-    </row>
-    <row r="12" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+      <c r="Z11" s="1"/>
+      <c r="AA11" s="1"/>
+    </row>
+    <row r="12" spans="1:27" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2062,7 +2131,7 @@
         <v>16</v>
       </c>
       <c r="G12" s="32"/>
-      <c r="H12" s="46" t="s">
+      <c r="H12" s="40" t="s">
         <v>17</v>
       </c>
       <c r="I12" s="1"/>
@@ -2072,8 +2141,20 @@
       <c r="M12" s="1"/>
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
-    </row>
-    <row r="13" spans="1:15" ht="23" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+      <c r="Z12" s="1"/>
+      <c r="AA12" s="1"/>
+    </row>
+    <row r="13" spans="1:27" ht="22.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2085,7 +2166,7 @@
         <v>20</v>
       </c>
       <c r="G13" s="32"/>
-      <c r="H13" s="46" t="s">
+      <c r="H13" s="40" t="s">
         <v>18</v>
       </c>
       <c r="I13" s="1"/>
@@ -2095,8 +2176,20 @@
       <c r="M13" s="1"/>
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
-    </row>
-    <row r="14" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+      <c r="Z13" s="1"/>
+      <c r="AA13" s="1"/>
+    </row>
+    <row r="14" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2108,7 +2201,7 @@
         <v>21</v>
       </c>
       <c r="G14" s="32"/>
-      <c r="H14" s="46" t="s">
+      <c r="H14" s="40" t="s">
         <v>22</v>
       </c>
       <c r="I14" s="1"/>
@@ -2118,8 +2211,20 @@
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
-    </row>
-    <row r="15" spans="1:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+      <c r="Z14" s="1"/>
+      <c r="AA14" s="1"/>
+    </row>
+    <row r="15" spans="1:27" ht="19.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2131,7 +2236,7 @@
         <v>9</v>
       </c>
       <c r="G15" s="32"/>
-      <c r="H15" s="46" t="s">
+      <c r="H15" s="40" t="s">
         <v>23</v>
       </c>
       <c r="I15" s="1"/>
@@ -2141,8 +2246,20 @@
       <c r="M15" s="1"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
-    </row>
-    <row r="16" spans="1:15" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="P15" s="1"/>
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+      <c r="Z15" s="1"/>
+      <c r="AA15" s="1"/>
+    </row>
+    <row r="16" spans="1:27" ht="10.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2158,8 +2275,20 @@
       <c r="M16" s="1"/>
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
-    </row>
-    <row r="17" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+      <c r="Z16" s="1"/>
+      <c r="AA16" s="1"/>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2175,8 +2304,20 @@
       <c r="M17" s="1"/>
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
-    </row>
-    <row r="18" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+      <c r="Z17" s="1"/>
+      <c r="AA17" s="1"/>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2192,8 +2333,20 @@
       <c r="M18" s="1"/>
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
-    </row>
-    <row r="19" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P18" s="1"/>
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+      <c r="Z18" s="1"/>
+      <c r="AA18" s="1"/>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2209,8 +2362,20 @@
       <c r="M19" s="1"/>
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
-    </row>
-    <row r="20" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P19" s="1"/>
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+      <c r="Z19" s="1"/>
+      <c r="AA19" s="1"/>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2226,8 +2391,20 @@
       <c r="M20" s="1"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
-    </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P20" s="1"/>
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+      <c r="Z20" s="1"/>
+      <c r="AA20" s="1"/>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2243,8 +2420,20 @@
       <c r="M21" s="1"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
-    </row>
-    <row r="22" spans="1:15" x14ac:dyDescent="0.35">
+      <c r="P21" s="1"/>
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+      <c r="Z21" s="1"/>
+      <c r="AA21" s="1"/>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2260,6 +2449,424 @@
       <c r="M22" s="1"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
+      <c r="P22" s="1"/>
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+      <c r="Z22" s="1"/>
+      <c r="AA22" s="1"/>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A23" s="1"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
+      <c r="D23" s="1"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
+      <c r="J23" s="1"/>
+      <c r="K23" s="1"/>
+      <c r="L23" s="1"/>
+      <c r="M23" s="1"/>
+      <c r="N23" s="1"/>
+      <c r="O23" s="1"/>
+      <c r="P23" s="1"/>
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+      <c r="Z23" s="1"/>
+      <c r="AA23" s="1"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A24" s="1"/>
+      <c r="B24" s="1"/>
+      <c r="C24" s="1"/>
+      <c r="D24" s="1"/>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+      <c r="I24" s="1"/>
+      <c r="J24" s="1"/>
+      <c r="K24" s="1"/>
+      <c r="L24" s="1"/>
+      <c r="M24" s="1"/>
+      <c r="N24" s="1"/>
+      <c r="O24" s="1"/>
+      <c r="P24" s="1"/>
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+      <c r="Z24" s="1"/>
+      <c r="AA24" s="1"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A25" s="1"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
+      <c r="J25" s="1"/>
+      <c r="K25" s="1"/>
+      <c r="L25" s="1"/>
+      <c r="M25" s="1"/>
+      <c r="N25" s="1"/>
+      <c r="O25" s="1"/>
+      <c r="P25" s="1"/>
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+      <c r="Z25" s="1"/>
+      <c r="AA25" s="1"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A26" s="1"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
+      <c r="D26" s="1"/>
+      <c r="E26" s="1"/>
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+      <c r="I26" s="1"/>
+      <c r="J26" s="1"/>
+      <c r="K26" s="1"/>
+      <c r="L26" s="1"/>
+      <c r="M26" s="1"/>
+      <c r="N26" s="1"/>
+      <c r="O26" s="1"/>
+      <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+      <c r="Z26" s="1"/>
+      <c r="AA26" s="1"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
+      <c r="AA27" s="1"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+      <c r="Z28" s="1"/>
+      <c r="AA28" s="1"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+      <c r="Z29" s="1"/>
+      <c r="AA29" s="1"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+      <c r="Z30" s="1"/>
+      <c r="AA30" s="1"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+      <c r="Z31" s="1"/>
+      <c r="AA31" s="1"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+      <c r="Z32" s="1"/>
+      <c r="AA32" s="1"/>
+    </row>
+    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+      <c r="Z33" s="1"/>
+      <c r="AA33" s="1"/>
+    </row>
+    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+      <c r="Z34" s="1"/>
+      <c r="AA34" s="1"/>
+    </row>
+    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+      <c r="Y35" s="1"/>
+      <c r="Z35" s="1"/>
+      <c r="AA35" s="1"/>
+    </row>
+    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+      <c r="Z36" s="1"/>
+      <c r="AA36" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2273,25 +2880,25 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2C21F710-274B-4FE8-B318-9DF41288548A}">
-  <dimension ref="A1:P26"/>
+  <dimension ref="A1:Y40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2.453125" customWidth="1"/>
-    <col min="2" max="2" width="13.6328125" customWidth="1"/>
-    <col min="3" max="3" width="19.453125" customWidth="1"/>
-    <col min="4" max="4" width="1.81640625" customWidth="1"/>
-    <col min="5" max="5" width="18.7265625" customWidth="1"/>
-    <col min="6" max="6" width="2.1796875" customWidth="1"/>
+    <col min="1" max="1" width="2.44140625" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.44140625" customWidth="1"/>
+    <col min="4" max="4" width="1.77734375" customWidth="1"/>
+    <col min="5" max="5" width="18.77734375" customWidth="1"/>
+    <col min="6" max="6" width="2.21875" customWidth="1"/>
     <col min="7" max="7" width="20" customWidth="1"/>
     <col min="8" max="8" width="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:25" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
@@ -2308,8 +2915,17 @@
       <c r="N1" s="1"/>
       <c r="O1" s="1"/>
       <c r="P1" s="1"/>
-    </row>
-    <row r="2" spans="1:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1"/>
+      <c r="S1" s="1"/>
+      <c r="T1" s="1"/>
+      <c r="U1" s="1"/>
+      <c r="V1" s="1"/>
+      <c r="W1" s="1"/>
+      <c r="X1" s="1"/>
+      <c r="Y1" s="1"/>
+    </row>
+    <row r="2" spans="1:25" ht="18" x14ac:dyDescent="0.35">
       <c r="A2" s="1"/>
       <c r="B2" s="13"/>
       <c r="C2" s="25" t="s">
@@ -2332,21 +2948,24 @@
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
       <c r="P2" s="1"/>
-    </row>
-    <row r="3" spans="1:16" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="Q2" s="1"/>
+      <c r="R2" s="1"/>
+      <c r="S2" s="1"/>
+      <c r="T2" s="1"/>
+      <c r="U2" s="1"/>
+      <c r="V2" s="1"/>
+      <c r="W2" s="1"/>
+      <c r="X2" s="1"/>
+      <c r="Y2" s="1"/>
+    </row>
+    <row r="3" spans="1:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A3" s="1"/>
       <c r="B3" s="15"/>
-      <c r="C3" s="28" t="s">
-        <v>8</v>
-      </c>
+      <c r="C3" s="28"/>
       <c r="D3" s="29"/>
-      <c r="E3" s="28" t="s">
-        <v>21</v>
-      </c>
+      <c r="E3" s="28"/>
       <c r="F3" s="30"/>
-      <c r="G3" s="28" t="s">
-        <v>13</v>
-      </c>
+      <c r="G3" s="28"/>
       <c r="H3" s="11"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
@@ -2356,23 +2975,26 @@
       <c r="N3" s="1"/>
       <c r="O3" s="1"/>
       <c r="P3" s="1"/>
-    </row>
-    <row r="4" spans="1:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="Q3" s="1"/>
+      <c r="R3" s="1"/>
+      <c r="S3" s="1"/>
+      <c r="T3" s="1"/>
+      <c r="U3" s="1"/>
+      <c r="V3" s="1"/>
+      <c r="W3" s="1"/>
+      <c r="X3" s="1"/>
+      <c r="Y3" s="1"/>
+    </row>
+    <row r="4" spans="1:25" ht="18" x14ac:dyDescent="0.35">
       <c r="A4" s="1"/>
       <c r="B4" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="18">
-        <v>1700000</v>
-      </c>
+      <c r="C4" s="18"/>
       <c r="D4" s="19"/>
-      <c r="E4" s="18">
-        <v>0</v>
-      </c>
+      <c r="E4" s="18"/>
       <c r="F4" s="23"/>
-      <c r="G4" s="14">
-        <v>166</v>
-      </c>
+      <c r="G4" s="14"/>
       <c r="H4" s="10"/>
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
@@ -2382,23 +3004,26 @@
       <c r="N4" s="1"/>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
-    </row>
-    <row r="5" spans="1:16" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="Q4" s="1"/>
+      <c r="R4" s="1"/>
+      <c r="S4" s="1"/>
+      <c r="T4" s="1"/>
+      <c r="U4" s="1"/>
+      <c r="V4" s="1"/>
+      <c r="W4" s="1"/>
+      <c r="X4" s="1"/>
+      <c r="Y4" s="1"/>
+    </row>
+    <row r="5" spans="1:25" ht="18" x14ac:dyDescent="0.35">
       <c r="A5" s="1"/>
       <c r="B5" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="18">
-        <v>9400000</v>
-      </c>
+      <c r="C5" s="18"/>
       <c r="D5" s="19"/>
-      <c r="E5" s="18">
-        <v>3080000</v>
-      </c>
+      <c r="E5" s="18"/>
       <c r="F5" s="23"/>
-      <c r="G5" s="18">
-        <v>7210000</v>
-      </c>
+      <c r="G5" s="18"/>
       <c r="H5" s="12"/>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -2408,23 +3033,26 @@
       <c r="N5" s="1"/>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
-    </row>
-    <row r="6" spans="1:16" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1"/>
+      <c r="S5" s="1"/>
+      <c r="T5" s="1"/>
+      <c r="U5" s="1"/>
+      <c r="V5" s="1"/>
+      <c r="W5" s="1"/>
+      <c r="X5" s="1"/>
+      <c r="Y5" s="1"/>
+    </row>
+    <row r="6" spans="1:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
       <c r="B6" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="18">
-        <v>4600000</v>
-      </c>
+      <c r="C6" s="18"/>
       <c r="D6" s="19"/>
-      <c r="E6" s="18">
-        <v>2300000</v>
-      </c>
+      <c r="E6" s="18"/>
       <c r="F6" s="23"/>
-      <c r="G6" s="16">
-        <v>4800000</v>
-      </c>
+      <c r="G6" s="16"/>
       <c r="H6" s="11"/>
       <c r="I6" s="1"/>
       <c r="J6" s="1"/>
@@ -2434,28 +3062,37 @@
       <c r="N6" s="1"/>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
-    </row>
-    <row r="7" spans="1:16" ht="19" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1"/>
+      <c r="S6" s="1"/>
+      <c r="T6" s="1"/>
+      <c r="U6" s="1"/>
+      <c r="V6" s="1"/>
+      <c r="W6" s="1"/>
+      <c r="X6" s="1"/>
+      <c r="Y6" s="1"/>
+    </row>
+    <row r="7" spans="1:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A7" s="1"/>
       <c r="B7" s="20" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="21">
         <f>SUM(C4:C6)</f>
-        <v>15700000</v>
+        <v>0</v>
       </c>
       <c r="D7" s="22">
         <f>SUM(C4:C6)</f>
-        <v>15700000</v>
+        <v>0</v>
       </c>
       <c r="E7" s="21">
         <f>SUM(E4:E6)</f>
-        <v>5380000</v>
+        <v>0</v>
       </c>
       <c r="F7" s="24"/>
       <c r="G7" s="21">
         <f>SUM(G4:G6)</f>
-        <v>12010166</v>
+        <v>0</v>
       </c>
       <c r="H7" s="11"/>
       <c r="I7" s="1"/>
@@ -2466,8 +3103,17 @@
       <c r="N7" s="1"/>
       <c r="O7" s="1"/>
       <c r="P7" s="1"/>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1"/>
+      <c r="S7" s="1"/>
+      <c r="T7" s="1"/>
+      <c r="U7" s="1"/>
+      <c r="V7" s="1"/>
+      <c r="W7" s="1"/>
+      <c r="X7" s="1"/>
+      <c r="Y7" s="1"/>
+    </row>
+    <row r="8" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A8" s="1"/>
       <c r="B8" s="1"/>
       <c r="C8" s="1"/>
@@ -2484,8 +3130,17 @@
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
       <c r="P8" s="1"/>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1"/>
+      <c r="S8" s="1"/>
+      <c r="T8" s="1"/>
+      <c r="U8" s="1"/>
+      <c r="V8" s="1"/>
+      <c r="W8" s="1"/>
+      <c r="X8" s="1"/>
+      <c r="Y8" s="1"/>
+    </row>
+    <row r="9" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A9" s="1"/>
       <c r="B9" s="1"/>
       <c r="C9" s="1"/>
@@ -2502,8 +3157,17 @@
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
       <c r="P9" s="1"/>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1"/>
+      <c r="S9" s="1"/>
+      <c r="T9" s="1"/>
+      <c r="U9" s="1"/>
+      <c r="V9" s="1"/>
+      <c r="W9" s="1"/>
+      <c r="X9" s="1"/>
+      <c r="Y9" s="1"/>
+    </row>
+    <row r="10" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
@@ -2520,8 +3184,17 @@
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
       <c r="P10" s="1"/>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1"/>
+      <c r="S10" s="1"/>
+      <c r="T10" s="1"/>
+      <c r="U10" s="1"/>
+      <c r="V10" s="1"/>
+      <c r="W10" s="1"/>
+      <c r="X10" s="1"/>
+      <c r="Y10" s="1"/>
+    </row>
+    <row r="11" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
@@ -2538,8 +3211,17 @@
       <c r="N11" s="1"/>
       <c r="O11" s="1"/>
       <c r="P11" s="1"/>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q11" s="1"/>
+      <c r="R11" s="1"/>
+      <c r="S11" s="1"/>
+      <c r="T11" s="1"/>
+      <c r="U11" s="1"/>
+      <c r="V11" s="1"/>
+      <c r="W11" s="1"/>
+      <c r="X11" s="1"/>
+      <c r="Y11" s="1"/>
+    </row>
+    <row r="12" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
@@ -2556,8 +3238,17 @@
       <c r="N12" s="1"/>
       <c r="O12" s="1"/>
       <c r="P12" s="1"/>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q12" s="1"/>
+      <c r="R12" s="1"/>
+      <c r="S12" s="1"/>
+      <c r="T12" s="1"/>
+      <c r="U12" s="1"/>
+      <c r="V12" s="1"/>
+      <c r="W12" s="1"/>
+      <c r="X12" s="1"/>
+      <c r="Y12" s="1"/>
+    </row>
+    <row r="13" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
@@ -2574,8 +3265,17 @@
       <c r="N13" s="1"/>
       <c r="O13" s="1"/>
       <c r="P13" s="1"/>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q13" s="1"/>
+      <c r="R13" s="1"/>
+      <c r="S13" s="1"/>
+      <c r="T13" s="1"/>
+      <c r="U13" s="1"/>
+      <c r="V13" s="1"/>
+      <c r="W13" s="1"/>
+      <c r="X13" s="1"/>
+      <c r="Y13" s="1"/>
+    </row>
+    <row r="14" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -2592,8 +3292,17 @@
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q14" s="1"/>
+      <c r="R14" s="1"/>
+      <c r="S14" s="1"/>
+      <c r="T14" s="1"/>
+      <c r="U14" s="1"/>
+      <c r="V14" s="1"/>
+      <c r="W14" s="1"/>
+      <c r="X14" s="1"/>
+      <c r="Y14" s="1"/>
+    </row>
+    <row r="15" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -2610,8 +3319,17 @@
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q15" s="1"/>
+      <c r="R15" s="1"/>
+      <c r="S15" s="1"/>
+      <c r="T15" s="1"/>
+      <c r="U15" s="1"/>
+      <c r="V15" s="1"/>
+      <c r="W15" s="1"/>
+      <c r="X15" s="1"/>
+      <c r="Y15" s="1"/>
+    </row>
+    <row r="16" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -2628,8 +3346,17 @@
       <c r="N16" s="1"/>
       <c r="O16" s="1"/>
       <c r="P16" s="1"/>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="1"/>
+      <c r="T16" s="1"/>
+      <c r="U16" s="1"/>
+      <c r="V16" s="1"/>
+      <c r="W16" s="1"/>
+      <c r="X16" s="1"/>
+      <c r="Y16" s="1"/>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -2646,8 +3373,17 @@
       <c r="N17" s="1"/>
       <c r="O17" s="1"/>
       <c r="P17" s="1"/>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q17" s="1"/>
+      <c r="R17" s="1"/>
+      <c r="S17" s="1"/>
+      <c r="T17" s="1"/>
+      <c r="U17" s="1"/>
+      <c r="V17" s="1"/>
+      <c r="W17" s="1"/>
+      <c r="X17" s="1"/>
+      <c r="Y17" s="1"/>
+    </row>
+    <row r="18" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -2664,8 +3400,17 @@
       <c r="N18" s="1"/>
       <c r="O18" s="1"/>
       <c r="P18" s="1"/>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q18" s="1"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="1"/>
+      <c r="T18" s="1"/>
+      <c r="U18" s="1"/>
+      <c r="V18" s="1"/>
+      <c r="W18" s="1"/>
+      <c r="X18" s="1"/>
+      <c r="Y18" s="1"/>
+    </row>
+    <row r="19" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -2682,8 +3427,17 @@
       <c r="N19" s="1"/>
       <c r="O19" s="1"/>
       <c r="P19" s="1"/>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q19" s="1"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="1"/>
+      <c r="T19" s="1"/>
+      <c r="U19" s="1"/>
+      <c r="V19" s="1"/>
+      <c r="W19" s="1"/>
+      <c r="X19" s="1"/>
+      <c r="Y19" s="1"/>
+    </row>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -2700,8 +3454,17 @@
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q20" s="1"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="1"/>
+      <c r="T20" s="1"/>
+      <c r="U20" s="1"/>
+      <c r="V20" s="1"/>
+      <c r="W20" s="1"/>
+      <c r="X20" s="1"/>
+      <c r="Y20" s="1"/>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -2718,8 +3481,17 @@
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q21" s="1"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="1"/>
+      <c r="T21" s="1"/>
+      <c r="U21" s="1"/>
+      <c r="V21" s="1"/>
+      <c r="W21" s="1"/>
+      <c r="X21" s="1"/>
+      <c r="Y21" s="1"/>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -2736,8 +3508,17 @@
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q22" s="1"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="1"/>
+      <c r="T22" s="1"/>
+      <c r="U22" s="1"/>
+      <c r="V22" s="1"/>
+      <c r="W22" s="1"/>
+      <c r="X22" s="1"/>
+      <c r="Y22" s="1"/>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -2754,8 +3535,17 @@
       <c r="N23" s="1"/>
       <c r="O23" s="1"/>
       <c r="P23" s="1"/>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q23" s="1"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="1"/>
+      <c r="T23" s="1"/>
+      <c r="U23" s="1"/>
+      <c r="V23" s="1"/>
+      <c r="W23" s="1"/>
+      <c r="X23" s="1"/>
+      <c r="Y23" s="1"/>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -2772,8 +3562,17 @@
       <c r="N24" s="1"/>
       <c r="O24" s="1"/>
       <c r="P24" s="1"/>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q24" s="1"/>
+      <c r="R24" s="1"/>
+      <c r="S24" s="1"/>
+      <c r="T24" s="1"/>
+      <c r="U24" s="1"/>
+      <c r="V24" s="1"/>
+      <c r="W24" s="1"/>
+      <c r="X24" s="1"/>
+      <c r="Y24" s="1"/>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -2790,8 +3589,17 @@
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q25" s="1"/>
+      <c r="R25" s="1"/>
+      <c r="S25" s="1"/>
+      <c r="T25" s="1"/>
+      <c r="U25" s="1"/>
+      <c r="V25" s="1"/>
+      <c r="W25" s="1"/>
+      <c r="X25" s="1"/>
+      <c r="Y25" s="1"/>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.3">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -2808,6 +3616,393 @@
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
+      <c r="Q26" s="1"/>
+      <c r="R26" s="1"/>
+      <c r="S26" s="1"/>
+      <c r="T26" s="1"/>
+      <c r="U26" s="1"/>
+      <c r="V26" s="1"/>
+      <c r="W26" s="1"/>
+      <c r="X26" s="1"/>
+      <c r="Y26" s="1"/>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A27" s="1"/>
+      <c r="B27" s="1"/>
+      <c r="C27" s="1"/>
+      <c r="D27" s="1"/>
+      <c r="E27" s="1"/>
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1"/>
+      <c r="M27" s="1"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+    </row>
+    <row r="28" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A28" s="1"/>
+      <c r="B28" s="1"/>
+      <c r="C28" s="1"/>
+      <c r="D28" s="1"/>
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1"/>
+      <c r="M28" s="1"/>
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1"/>
+      <c r="R28" s="1"/>
+      <c r="S28" s="1"/>
+      <c r="T28" s="1"/>
+      <c r="U28" s="1"/>
+      <c r="V28" s="1"/>
+      <c r="W28" s="1"/>
+      <c r="X28" s="1"/>
+      <c r="Y28" s="1"/>
+    </row>
+    <row r="29" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A29" s="1"/>
+      <c r="B29" s="1"/>
+      <c r="C29" s="1"/>
+      <c r="D29" s="1"/>
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1"/>
+      <c r="M29" s="1"/>
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1"/>
+      <c r="R29" s="1"/>
+      <c r="S29" s="1"/>
+      <c r="T29" s="1"/>
+      <c r="U29" s="1"/>
+      <c r="V29" s="1"/>
+      <c r="W29" s="1"/>
+      <c r="X29" s="1"/>
+      <c r="Y29" s="1"/>
+    </row>
+    <row r="30" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A30" s="1"/>
+      <c r="B30" s="1"/>
+      <c r="C30" s="1"/>
+      <c r="D30" s="1"/>
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1"/>
+      <c r="L30" s="1"/>
+      <c r="M30" s="1"/>
+      <c r="N30" s="1"/>
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1"/>
+      <c r="R30" s="1"/>
+      <c r="S30" s="1"/>
+      <c r="T30" s="1"/>
+      <c r="U30" s="1"/>
+      <c r="V30" s="1"/>
+      <c r="W30" s="1"/>
+      <c r="X30" s="1"/>
+      <c r="Y30" s="1"/>
+    </row>
+    <row r="31" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A31" s="1"/>
+      <c r="B31" s="1"/>
+      <c r="C31" s="1"/>
+      <c r="D31" s="1"/>
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1"/>
+      <c r="L31" s="1"/>
+      <c r="M31" s="1"/>
+      <c r="N31" s="1"/>
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="1"/>
+      <c r="T31" s="1"/>
+      <c r="U31" s="1"/>
+      <c r="V31" s="1"/>
+      <c r="W31" s="1"/>
+      <c r="X31" s="1"/>
+      <c r="Y31" s="1"/>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A32" s="1"/>
+      <c r="B32" s="1"/>
+      <c r="C32" s="1"/>
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1"/>
+      <c r="M32" s="1"/>
+      <c r="N32" s="1"/>
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1"/>
+      <c r="R32" s="1"/>
+      <c r="S32" s="1"/>
+      <c r="T32" s="1"/>
+      <c r="U32" s="1"/>
+      <c r="V32" s="1"/>
+      <c r="W32" s="1"/>
+      <c r="X32" s="1"/>
+      <c r="Y32" s="1"/>
+    </row>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A33" s="1"/>
+      <c r="B33" s="1"/>
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="1"/>
+      <c r="T33" s="1"/>
+      <c r="U33" s="1"/>
+      <c r="V33" s="1"/>
+      <c r="W33" s="1"/>
+      <c r="X33" s="1"/>
+      <c r="Y33" s="1"/>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A34" s="1"/>
+      <c r="B34" s="1"/>
+      <c r="C34" s="1"/>
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1"/>
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1"/>
+      <c r="R34" s="1"/>
+      <c r="S34" s="1"/>
+      <c r="T34" s="1"/>
+      <c r="U34" s="1"/>
+      <c r="V34" s="1"/>
+      <c r="W34" s="1"/>
+      <c r="X34" s="1"/>
+      <c r="Y34" s="1"/>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A35" s="1"/>
+      <c r="B35" s="1"/>
+      <c r="C35" s="1"/>
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+      <c r="K35" s="1"/>
+      <c r="L35" s="1"/>
+      <c r="M35" s="1"/>
+      <c r="N35" s="1"/>
+      <c r="O35" s="1"/>
+      <c r="P35" s="1"/>
+      <c r="Q35" s="1"/>
+      <c r="R35" s="1"/>
+      <c r="S35" s="1"/>
+      <c r="T35" s="1"/>
+      <c r="U35" s="1"/>
+      <c r="V35" s="1"/>
+      <c r="W35" s="1"/>
+      <c r="X35" s="1"/>
+      <c r="Y35" s="1"/>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A36" s="1"/>
+      <c r="B36" s="1"/>
+      <c r="C36" s="1"/>
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+      <c r="K36" s="1"/>
+      <c r="L36" s="1"/>
+      <c r="M36" s="1"/>
+      <c r="N36" s="1"/>
+      <c r="O36" s="1"/>
+      <c r="P36" s="1"/>
+      <c r="Q36" s="1"/>
+      <c r="R36" s="1"/>
+      <c r="S36" s="1"/>
+      <c r="T36" s="1"/>
+      <c r="U36" s="1"/>
+      <c r="V36" s="1"/>
+      <c r="W36" s="1"/>
+      <c r="X36" s="1"/>
+      <c r="Y36" s="1"/>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A37" s="1"/>
+      <c r="B37" s="1"/>
+      <c r="C37" s="1"/>
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1"/>
+      <c r="N37" s="1"/>
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1"/>
+      <c r="R37" s="1"/>
+      <c r="S37" s="1"/>
+      <c r="T37" s="1"/>
+      <c r="U37" s="1"/>
+      <c r="V37" s="1"/>
+      <c r="W37" s="1"/>
+      <c r="X37" s="1"/>
+      <c r="Y37" s="1"/>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A38" s="1"/>
+      <c r="B38" s="1"/>
+      <c r="C38" s="1"/>
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1"/>
+      <c r="L38" s="1"/>
+      <c r="M38" s="1"/>
+      <c r="N38" s="1"/>
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="1"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="1"/>
+      <c r="V38" s="1"/>
+      <c r="W38" s="1"/>
+      <c r="X38" s="1"/>
+      <c r="Y38" s="1"/>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A39" s="1"/>
+      <c r="B39" s="1"/>
+      <c r="C39" s="1"/>
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+      <c r="K39" s="1"/>
+      <c r="L39" s="1"/>
+      <c r="M39" s="1"/>
+      <c r="N39" s="1"/>
+      <c r="O39" s="1"/>
+      <c r="P39" s="1"/>
+      <c r="Q39" s="1"/>
+      <c r="R39" s="1"/>
+      <c r="S39" s="1"/>
+      <c r="T39" s="1"/>
+      <c r="U39" s="1"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="1"/>
+      <c r="X39" s="1"/>
+      <c r="Y39" s="1"/>
+    </row>
+    <row r="40" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+      <c r="V40" s="1"/>
+      <c r="W40" s="1"/>
+      <c r="X40" s="1"/>
+      <c r="Y40" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>